<commit_message>
All practice till 16th Oct 2023
</commit_message>
<xml_diff>
--- a/Project_Timeline/Timeline.xlsx
+++ b/Project_Timeline/Timeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://servicenow-my.sharepoint.com/personal/yogesh_shinde_servicenow_com/Documents/Learning &amp; Development/Python_Dev/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://servicenow-my.sharepoint.com/personal/yogesh_shinde_servicenow_com/Documents/Learning &amp; Development/Dev_Public/Project_Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{45978271-2888-2748-BE49-5CE047777AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3D321A3-995A-CC44-B8F1-577014E0B1A1}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{45978271-2888-2748-BE49-5CE047777AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11126076-3E9D-B34F-B7ED-03AD130CC436}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{B8F8EECD-E04F-934C-9DA1-12B10D7679D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Activity</t>
   </si>
@@ -66,6 +66,24 @@
   </si>
   <si>
     <t>Close</t>
+  </si>
+  <si>
+    <t>% Complete</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>In_Progress</t>
+  </si>
+  <si>
+    <t>Not_Started</t>
+  </si>
+  <si>
+    <t>On_Hold</t>
   </si>
 </sst>
 </file>
@@ -74,7 +92,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,10 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D10CDBB-EA1B-CB40-B301-2FF440A821A6}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,7 +460,7 @@
     <col min="2" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,8 +470,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -463,8 +488,14 @@
         <f>B2+10</f>
         <v>45180</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -476,21 +507,33 @@
         <f>B3+10</f>
         <v>45191</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B6" si="0">C3+1</f>
+        <f t="shared" ref="B4:B5" si="0">C3+1</f>
         <v>45192</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C6" si="1">B4+10</f>
+        <f t="shared" ref="C4:C5" si="1">B4+10</f>
         <v>45202</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -502,8 +545,14 @@
         <f t="shared" si="1"/>
         <v>45213</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -515,8 +564,14 @@
         <f t="shared" ref="C6:C8" si="3">B6+10</f>
         <v>45224</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -528,8 +583,14 @@
         <f t="shared" si="3"/>
         <v>45235</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -540,6 +601,12 @@
       <c r="C8" s="2">
         <f t="shared" si="3"/>
         <v>45246</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>